<commit_message>
Added coockie clicker boot
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -511,17 +511,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -536,12 +536,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>35:6</t>
+          <t>44:14</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>47</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -551,12 +551,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -581,32 +581,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Real Madryt</t>
+          <t>AC Milan</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>36:16</t>
+          <t>35:20</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -651,37 +651,37 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Inter</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>26:18</t>
+          <t>38:24</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>37</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
     </row>
@@ -721,17 +721,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Atl. Madryt</t>
+          <t>Lazio</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -741,32 +741,32 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>24:16</t>
+          <t>31:15</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>34</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
     </row>
@@ -791,17 +791,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>Atalanta</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -811,22 +811,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>34:20</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>34</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -861,17 +861,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Betis</t>
+          <t>AS Roma</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -886,12 +886,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>23:16</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>34</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
     </row>
@@ -931,52 +931,52 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Osasuna</t>
+          <t>Udinese</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>26:21</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>25</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
     </row>
@@ -1001,37 +1001,37 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ath. Bilbao</t>
+          <t>Torino</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>25:17</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>23</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1051,12 +1051,12 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
     </row>
@@ -1071,47 +1071,47 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Vallecano</t>
+          <t>Fiorentina</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>24:20</t>
+          <t>21:24</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>23</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1141,17 +1141,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Mallorca</t>
+          <t>Juventus</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1161,12 +1161,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>14:16</t>
+          <t>27:12</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1211,37 +1211,37 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Girona</t>
+          <t>Bologna</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>26:27</t>
+          <t>23:29</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1251,12 +1251,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
     </row>
@@ -1281,12 +1281,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Empoli</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1296,42 +1296,42 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>23:18</t>
+          <t>16:22</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>22</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1351,17 +1351,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Almeria</t>
+          <t>Monza</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1376,22 +1376,22 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>18:26</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>21</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1421,42 +1421,42 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Espanyol</t>
+          <t>Lecce</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0:0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>21:26</t>
-        </is>
-      </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>?</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1471,12 +1471,12 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
     </row>
@@ -1491,12 +1491,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Getafe</t>
+          <t>Spezia</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,32 +1516,32 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>16:24</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>W</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1561,12 +1561,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Celta Vigo</t>
+          <t>Salernitana</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1586,32 +1586,32 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>23:35</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1631,22 +1631,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Valladolid</t>
+          <t>Sassuolo</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1656,12 +1656,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>13:25</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>R</t>
         </is>
       </c>
     </row>
@@ -1701,62 +1701,62 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Cadiz</t>
+          <t>Verona</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0:0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>12:28</t>
+          <t>13</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15:31</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>?</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
     </row>
@@ -1771,37 +1771,37 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>Sampdoria</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>17:26</t>
+          <t>8:31</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1811,12 +1811,12 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>W</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
     </row>
@@ -1841,12 +1841,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Elche</t>
+          <t>Cremonese</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1856,27 +1856,27 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1896,7 +1896,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>R</t>
         </is>
       </c>
     </row>

</xml_diff>